<commit_message>
Gift Log changes - 28th Apr 2023
</commit_message>
<xml_diff>
--- a/TestData/T1516_GiftLog_ClientGiftPre_ApprovalPage_RecipientsExceedsYearlyGiftAllowance.xlsx
+++ b/TestData/T1516_GiftLog_ClientGiftPre_ApprovalPage_RecipientsExceedsYearlyGiftAllowance.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515EA70D-8722-4379-81C1-A14031FA03BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59CA395-12E1-403B-B3E8-3A39EF517C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="6804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GiftLog" sheetId="4" r:id="rId1"/>
-    <sheet name="GiftLog_Currency" sheetId="6" r:id="rId2"/>
-    <sheet name="Users" sheetId="5" r:id="rId3"/>
+    <sheet name="Contact" sheetId="7" r:id="rId2"/>
+    <sheet name="ContactTypes" sheetId="8" r:id="rId3"/>
+    <sheet name="GiftLog_Currency" sheetId="6" r:id="rId4"/>
+    <sheet name="Users" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
   <si>
     <t>Client Gift Pre-approval</t>
   </si>
@@ -165,13 +167,46 @@
   </si>
   <si>
     <t>110.0</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>ContactTypesValue</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>External</t>
+  </si>
+  <si>
+    <t>testlast@mailinator.com</t>
+  </si>
+  <si>
+    <t>(541) 754-3010</t>
+  </si>
+  <si>
+    <t>External Contact</t>
+  </si>
+  <si>
+    <t>ContactType</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +218,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -205,18 +248,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -497,7 +543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -612,6 +658,89 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71607737-C7C9-466B-B424-409215616E00}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{85D8D10C-8F43-44DD-B02A-C7DBB2BD84A9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C674870-7E16-4E86-8A92-4D6617DAF46E}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -713,7 +842,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>

</xml_diff>